<commit_message>
prepared visualizations for the thesis
</commit_message>
<xml_diff>
--- a/performance_evaluation/validation_dataset.xlsx
+++ b/performance_evaluation/validation_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/zxowg46_s-cloud_uni-tuebingen_de/Documents/Thesis/esg_extraction/performance_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F765D065-3E40-40CE-9531-103304607D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4A88A9A-5F4D-4711-930F-EBA783922E84}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F765D065-3E40-40CE-9531-103304607D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{482E5F5E-B85A-40C2-8870-72F9B68AB50D}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1320,6 +1320,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1609,17 +1613,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67:E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.06640625" customWidth="1"/>
     <col min="2" max="2" width="6.53125" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="55.73046875" style="2" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" customWidth="1"/>
   </cols>
@@ -1641,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1658,7 +1663,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1675,7 +1680,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1692,7 +1697,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1709,7 +1714,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1726,7 +1731,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="156.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1743,7 +1748,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1760,7 +1765,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1782,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1794,7 +1799,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1811,7 +1816,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1828,7 +1833,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1845,7 +1850,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="128.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1862,7 +1867,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1879,7 +1884,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1896,7 +1901,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1913,7 +1918,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1947,7 +1952,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1964,7 +1969,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1981,7 +1986,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1998,7 +2003,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2015,7 +2020,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -2032,7 +2037,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2049,7 +2054,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -2066,7 +2071,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -2083,7 +2088,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -2100,7 +2105,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -2134,7 +2139,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2151,7 +2156,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2168,7 +2173,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" ht="128.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2185,7 +2190,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" ht="270.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2202,7 +2207,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2219,7 +2224,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2236,7 +2241,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2253,7 +2258,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2287,7 +2292,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -2304,7 +2309,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2326,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2338,7 +2343,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" ht="156.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2355,7 +2360,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" ht="128.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2372,7 +2377,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" ht="185.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -2389,7 +2394,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" ht="199.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="171" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" ht="171" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -2491,7 +2496,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" ht="199.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2508,7 +2513,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -2525,7 +2530,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -2542,7 +2547,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -2559,7 +2564,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -2576,7 +2581,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -2593,7 +2598,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -2610,7 +2615,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -2627,7 +2632,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2649,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -2678,7 +2683,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -2695,7 +2700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -2712,7 +2717,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="171" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" ht="171" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -2729,7 +2734,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -3852,7 +3857,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E131" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E131" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SchneiderElectric_2024"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>